<commit_message>
TDI data, distance matrix for all
</commit_message>
<xml_diff>
--- a/data/TDI_individual_clusters/TDI_L_2500_500.xlsx
+++ b/data/TDI_individual_clusters/TDI_L_2500_500.xlsx
@@ -15,6 +15,7 @@
     <sheet name="TDI_L_2500_500" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -3514,11 +3515,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1859236880"/>
-        <c:axId val="-1859251568"/>
+        <c:axId val="1370068496"/>
+        <c:axId val="1370066864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1859236880"/>
+        <c:axId val="1370068496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3616,7 +3617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1859251568"/>
+        <c:crossAx val="1370066864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3625,7 +3626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1859251568"/>
+        <c:axId val="1370066864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-4"/>
@@ -3734,7 +3735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1859236880"/>
+        <c:crossAx val="1370068496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4681,7 +4682,7 @@
   <dimension ref="A1:EW4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>